<commit_message>
removed unused buttons, improved formatting
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
@@ -153,7 +153,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +184,14 @@
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -562,17 +568,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -674,9 +669,6 @@
     <xf numFmtId="172" fontId="6" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="167" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -701,12 +693,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -801,9 +794,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 14:25:08</v>
+        <v>Paused at 16:47:29</v>
         <stp/>
-        <stp>{5888B409-8AEC-4D3F-8F0A-FDF5A326FF90}</stp>
+        <stp>{F656BE7C-EA5C-4778-B7AD-EAA35195443C}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -927,10 +920,6 @@
       <sheetName val="Swap3M"/>
       <sheetName val="Swap6M"/>
       <sheetName val="ON"/>
-      <sheetName val="1M (2)"/>
-      <sheetName val="3M (2)"/>
-      <sheetName val="6M (2)"/>
-      <sheetName val="1Y (2)"/>
       <sheetName val="1M (3)"/>
       <sheetName val="3M (4)"/>
       <sheetName val="6M (3)"/>
@@ -943,7 +932,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>103</v>
+            <v>1545</v>
           </cell>
         </row>
       </sheetData>
@@ -1050,53 +1039,25 @@
       <sheetData sheetId="17">
         <row r="6">
           <cell r="D6" t="str">
-            <v>6E</v>
+            <v>1E</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="18">
         <row r="6">
           <cell r="D6" t="str">
-            <v>6E</v>
+            <v>3E</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="19">
         <row r="6">
           <cell r="D6" t="str">
-            <v>3E</v>
+            <v>6E</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="20">
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>6E</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="21">
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>1E</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="22">
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>3E</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23">
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>6E</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="24">
         <row r="6">
           <cell r="D6" t="str">
             <v>12E</v>
@@ -1401,7 +1362,7 @@
   <dimension ref="A1:W60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1411,7 +1372,7 @@
     <col min="3" max="3" width="17.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="2.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -1454,7 +1415,7 @@
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="50" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9"/>
@@ -1468,9 +1429,7 @@
       <c r="H2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="40">
-        <v>41731.599895833337</v>
-      </c>
+      <c r="I2" s="40"/>
       <c r="J2" s="14"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1492,9 +1451,9 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>EURSTD</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="49">
         <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41731</v>
+        <v>41733</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18">
@@ -1506,12 +1465,12 @@
         <v/>
       </c>
       <c r="G3" s="12"/>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="47" t="str">
+      <c r="I3" s="46" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Paused at 14:25:08</v>
+        <v>Paused at 16:47:29</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="5"/>
@@ -1534,9 +1493,9 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>EURON</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="41">
         <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41731</v>
+        <v>41733</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18">
@@ -1548,11 +1507,11 @@
         <v/>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="46">
-        <v>142.93</v>
+      <c r="I4" s="45">
+        <v>143.4</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="5"/>
@@ -1575,9 +1534,9 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>EUR1M</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="41">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41733</v>
+        <v>41737</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="18">
@@ -1594,7 +1553,7 @@
       </c>
       <c r="I5" s="21">
         <f ca="1">[1]!TriggerCounter</f>
-        <v>103</v>
+        <v>1545</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="5"/>
@@ -1617,9 +1576,9 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>EUR3M</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="41">
         <f>C5</f>
-        <v>41733</v>
+        <v>41737</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
@@ -1636,7 +1595,7 @@
       </c>
       <c r="I6" s="21">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1449</v>
+        <v>2113</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5"/>
@@ -1653,15 +1612,15 @@
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="16" t="str">
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>EUR6M</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="41">
         <f>C6</f>
-        <v>41733</v>
+        <v>41737</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18">
@@ -1673,8 +1632,12 @@
         <v/>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
+      <c r="H7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>6</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1696,9 +1659,9 @@
         <f>UPPER(Currency)&amp;"1Y"</f>
         <v>EUR1Y</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="41">
         <f>C7</f>
-        <v>41733</v>
+        <v>41737</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18">
@@ -1710,11 +1673,12 @@
         <v/>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>6</v>
+      <c r="H8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="21">
+        <f>_xll.qlFunctionCount(Trigger)+_xll.ohFunctionCount(Trigger)</f>
+        <v>1016</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="5"/>
@@ -1734,9 +1698,9 @@
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="24"/>
-      <c r="C9" s="43">
+      <c r="C9" s="42">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41729</v>
+        <v>41731</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26" t="e">
@@ -1745,15 +1709,15 @@
       </c>
       <c r="F9" s="15" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for March 31st, 2014</v>
+        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 2nd, 2014</v>
       </c>
       <c r="G9" s="12"/>
-      <c r="H9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="21">
-        <f>_xll.qlFunctionCount(Trigger)+_xll.ohFunctionCount(Trigger)</f>
-        <v>1016</v>
+      <c r="H9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="23" t="str">
+        <f>_xll.ohBoostVersion(Trigger)</f>
+        <v>1_52</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="5"/>
@@ -1773,9 +1737,9 @@
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="44">
+      <c r="C10" s="43">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>41730</v>
+        <v>41732</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="29" t="e">
@@ -1784,15 +1748,15 @@
       </c>
       <c r="F10" s="19" t="str">
         <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 1st, 2014</v>
+        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 3rd, 2014</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I10" s="23" t="str">
-        <f>_xll.ohBoostVersion(Trigger)</f>
-        <v>1_52</v>
+        <f>_xll.qlVersion(Trigger)</f>
+        <v>1.4.1</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="5"/>
@@ -1809,32 +1773,32 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="27" t="str">
         <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor6M"</f>
         <v>Euribor6M</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <f>EvaluationDate</f>
-        <v>41731</v>
+        <v>41733</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="29">
         <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
-        <v>4.2300000000000003E-3</v>
+        <v>4.2699999999999995E-3</v>
       </c>
       <c r="F11" s="19" t="str">
         <f>IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
         <v/>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="23" t="str">
-        <f>_xll.qlVersion(Trigger)</f>
-        <v>1.4.1</v>
+      <c r="H11" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="35" t="str">
+        <f>_xll.ohVersion(Trigger)</f>
+        <v>1.4.0</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="5"/>
@@ -1854,27 +1818,22 @@
     <row r="12" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="45">
+      <c r="C12" s="44">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
         <v>41897</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="32">
         <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
-        <v>4.0984918818513247E-3</v>
+        <v>3.9466493817900848E-3</v>
       </c>
       <c r="F12" s="33" t="str">
         <f>IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>
         <v/>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="35" t="str">
-        <f>_xll.ohVersion(Trigger)</f>
-        <v>1.4.0</v>
-      </c>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
       <c r="J12" s="14"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -2923,8 +2882,6 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>

</xml_diff>

<commit_message>
fixed term structure reference date when the evaluation date is a non-business date
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
@@ -794,9 +794,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 16:47:29</v>
+        <v>Updated at 18:17:09</v>
         <stp/>
-        <stp>{F656BE7C-EA5C-4778-B7AD-EAA35195443C}</stp>
+        <stp>{82FCE125-6EFD-4929-B078-31E64BE8BFF5}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -932,7 +932,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>1545</v>
+            <v>2</v>
           </cell>
         </row>
       </sheetData>
@@ -975,7 +975,7 @@
       <sheetData sheetId="7">
         <row r="6">
           <cell r="D6" t="str">
-            <v>J4</v>
+            <v>K4</v>
           </cell>
         </row>
       </sheetData>
@@ -989,7 +989,7 @@
       <sheetData sheetId="9">
         <row r="6">
           <cell r="D6" t="str">
-            <v>J4</v>
+            <v>K4</v>
           </cell>
         </row>
       </sheetData>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:W60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="C1" s="3" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Mar  3 2014 10:58:57</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 18 2014 11:20:01</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1452,8 +1452,8 @@
         <v>EURSTD</v>
       </c>
       <c r="C3" s="49">
-        <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41733</v>
+        <f>_xll.qlCalendarAdjust("TARGET",_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
+        <v>41751</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="I3" s="46" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Paused at 16:47:29</v>
+        <v>Updated at 18:17:09</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="5"/>
@@ -1494,8 +1494,8 @@
         <v>EURON</v>
       </c>
       <c r="C4" s="41">
-        <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41733</v>
+        <f>EvaluationDate</f>
+        <v>41751</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18">
@@ -1511,7 +1511,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="45">
-        <v>143.4</v>
+        <v>143.76</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="5"/>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="C5" s="41">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41737</v>
+        <v>41753</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="18">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
-        <v>1</v>
+        <v>0.99999241284908746</v>
       </c>
       <c r="F5" s="19" t="str">
         <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
@@ -1552,8 +1552,8 @@
         <v>12</v>
       </c>
       <c r="I5" s="21">
-        <f ca="1">[1]!TriggerCounter</f>
-        <v>1545</v>
+        <f>[1]!TriggerCounter</f>
+        <v>2</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="5"/>
@@ -1578,12 +1578,12 @@
       </c>
       <c r="C6" s="41">
         <f>C5</f>
-        <v>41737</v>
+        <v>41753</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
         <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
-        <v>1</v>
+        <v>0.99998969897916701</v>
       </c>
       <c r="F6" s="19" t="str">
         <f>IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="I6" s="21">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>2113</v>
+        <v>2104</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5"/>
@@ -1620,12 +1620,12 @@
       </c>
       <c r="C7" s="41">
         <f>C6</f>
-        <v>41737</v>
+        <v>41753</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18">
         <f>_xll.qlYieldTSDiscount(B7,C7,,Trigger)</f>
-        <v>1</v>
+        <v>0.99998576334947431</v>
       </c>
       <c r="F7" s="19" t="str">
         <f>IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
@@ -1661,12 +1661,12 @@
       </c>
       <c r="C8" s="41">
         <f>C7</f>
-        <v>41737</v>
+        <v>41753</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18">
         <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
-        <v>1</v>
+        <v>0.99998139728612334</v>
       </c>
       <c r="F8" s="19" t="str">
         <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
@@ -1700,7 +1700,7 @@
       <c r="B9" s="24"/>
       <c r="C9" s="42">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41731</v>
+        <v>41745</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26" t="e">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F9" s="15" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 2nd, 2014</v>
+        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 16th, 2014</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="22" t="s">
@@ -1739,16 +1739,16 @@
       <c r="B10" s="27"/>
       <c r="C10" s="43">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>41732</v>
+        <v>41746</v>
       </c>
       <c r="D10" s="36"/>
-      <c r="E10" s="29" t="e">
+      <c r="E10" s="29">
         <f>_xll.qlIndexFixing(FirstIndex,C10)</f>
-        <v>#NUM!</v>
+        <v>4.2599999999999999E-3</v>
       </c>
       <c r="F10" s="19" t="str">
-        <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v>qlIndexFixing - Missing Euribor6M Actual/360 fixing for April 3rd, 2014</v>
+        <f>IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
+        <v/>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="22" t="s">
@@ -1781,12 +1781,12 @@
       </c>
       <c r="C11" s="43">
         <f>EvaluationDate</f>
-        <v>41733</v>
+        <v>41751</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="29">
         <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
-        <v>4.2699999999999995E-3</v>
+        <v>4.3172221782871913E-3</v>
       </c>
       <c r="F11" s="19" t="str">
         <f>IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
@@ -1825,7 +1825,7 @@
       <c r="D12" s="31"/>
       <c r="E12" s="32">
         <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
-        <v>3.9466493817900848E-3</v>
+        <v>3.860561119210923E-3</v>
       </c>
       <c r="F12" s="33" t="str">
         <f>IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>

</xml_diff>

<commit_message>
EUR main checks: add fixings checks
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_MainChecks.xlsx
@@ -334,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -389,19 +389,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -515,30 +502,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -592,7 +555,7 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="62">
@@ -605,13 +568,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -619,31 +585,22 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -652,59 +609,53 @@
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -714,22 +665,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="8" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -826,28 +789,28 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 12:03:47</v>
+        <v>Updated at 15:21:51</v>
         <stp/>
-        <stp>{94744D71-80D7-4200-A1FC-40CACC119D7A}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:03:47</v>
-        <stp/>
-        <stp>{DF302822-A347-4205-9535-D9E7CE44E2D1}</stp>
+        <stp>{113A892D-4CD1-497F-B308-AA8CDA15A9EB}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:47</v>
+        <v>Updated at 15:21:29</v>
         <stp/>
-        <stp>{48A50FDF-53A5-4172-858A-3A9B641930D7}</stp>
+        <stp>{352F2324-65C4-4828-AF5D-EC90C2899719}</stp>
+        <tr r="Q6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:21:35</v>
+        <stp/>
+        <stp>{2CF6BBB2-90CB-473F-9E14-D20AAA4FD6E8}</stp>
         <tr r="P7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:32</v>
+        <v>Updated at 15:21:35</v>
         <stp/>
-        <stp>{A13EAEED-6F5B-411D-AFD3-AD290BD82324}</stp>
-        <tr r="Q6" s="2"/>
+        <stp>{BC086328-803A-407B-9494-67FD453A7587}</stp>
+        <tr r="Q7" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1239,7 +1202,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ103"/>
+  <dimension ref="A1:AJ104"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -1393,28 +1356,28 @@
       <c r="AJ3" s="3"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="46" t="s">
         <v>35</v>
       </c>
       <c r="I4" s="3"/>
@@ -1461,48 +1424,48 @@
       <c r="AJ4" s="3"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="49" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="26" t="str">
+      <c r="K5" s="24" t="str">
         <f>VLOOKUP(Currency,FuturesTable,3,0)</f>
         <v>FGBLc1</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="25">
         <v>41981</v>
       </c>
-      <c r="M5" s="28">
-        <v>150.68</v>
-      </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29" t="str">
+      <c r="M5" s="26">
+        <v>151.02000000000001</v>
+      </c>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 12:03:47</v>
+        <v>Updated at 15:21:51</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1532,47 +1495,47 @@
       <c r="AJ5" s="3"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="49" t="s">
         <v>36</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="22">
         <v>42170</v>
       </c>
-      <c r="M6" s="30">
-        <v>99.894999999999996</v>
-      </c>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31" t="str">
+      <c r="M6" s="28">
+        <v>99.915000000000006</v>
+      </c>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 12:03:32</v>
+        <v>Updated at 15:21:29</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1583,7 +1546,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>3258</v>
+        <v>2934</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1602,56 +1565,56 @@
       <c r="AJ6" s="3"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="49" t="s">
         <v>37</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="23" t="str">
+      <c r="K7" s="21" t="str">
         <f>Currency&amp;VLOOKUP(Currency,FuturesTable,5,0)&amp;VLOOKUP(Currency,FuturesTable,6,0)&amp;"10Y"</f>
         <v>EURAB6E10Y</v>
       </c>
-      <c r="L7" s="24">
-        <v>41929</v>
-      </c>
-      <c r="M7" s="33" t="str">
+      <c r="L7" s="22">
+        <v>41932</v>
+      </c>
+      <c r="M7" s="30" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>1.093/1.133</v>
-      </c>
-      <c r="N7" s="30">
-        <v>1.093</v>
-      </c>
-      <c r="O7" s="30">
-        <v>1.133</v>
-      </c>
-      <c r="P7" s="30" t="str">
+        <v>1.06/1.1</v>
+      </c>
+      <c r="N7" s="28">
+        <v>1.06</v>
+      </c>
+      <c r="O7" s="28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P7" s="28" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 12:03:47</v>
-      </c>
-      <c r="Q7" s="31" t="str">
+        <v>Updated at 15:21:35</v>
+      </c>
+      <c r="Q7" s="29" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 12:03:47</v>
+        <v>Updated at 15:21:35</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1676,28 +1639,28 @@
       <c r="AJ7" s="3"/>
     </row>
     <row r="8" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="49" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="3"/>
@@ -1734,28 +1697,28 @@
       <c r="AJ8" s="3"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="49" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="3"/>
@@ -1798,48 +1761,48 @@
       <c r="AJ9" s="3"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="49" t="s">
         <v>57</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="21" t="str">
+      <c r="K10" s="24" t="str">
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>Euribor6M</v>
       </c>
-      <c r="L10" s="22">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41929</v>
-      </c>
-      <c r="M10" s="32">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>1.8500000000000001E-3</v>
-      </c>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="34" t="str">
+      <c r="L10" s="25">
+        <f>_xll.qlCalendarAdvance("TARGET",L11,"-1M","f",,Trigger)</f>
+        <v>41904</v>
+      </c>
+      <c r="M10" s="58">
+        <f>_xll.qlIndexFixing(FirstIndex,L10,,Trigger)</f>
+        <v>1.8599999999999999E-3</v>
+      </c>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="59" t="str">
         <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
         <v/>
       </c>
@@ -1866,54 +1829,49 @@
       <c r="AJ10" s="3"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="49" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="23" t="str">
-        <f>UPPER(Currency)&amp;"STD"</f>
-        <v>EURSTD</v>
-      </c>
-      <c r="L11" s="24" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M11" s="25" t="e">
-        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="35" t="str">
-        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41932</v>
+      </c>
+      <c r="M11" s="60">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="61" t="str">
+        <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
         <v/>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="R11" s="8"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1934,43 +1892,43 @@
       <c r="AJ11" s="3"/>
     </row>
     <row r="12" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="58" t="s">
+      <c r="G12" s="53"/>
+      <c r="H12" s="54" t="s">
         <v>36</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="23" t="str">
-        <f>UPPER(Currency)&amp;"ON"</f>
-        <v>EURON</v>
-      </c>
-      <c r="L12" s="24" t="e">
+      <c r="K12" s="21" t="str">
+        <f>UPPER(Currency)&amp;"STD"</f>
+        <v>EURSTD</v>
+      </c>
+      <c r="L12" s="22">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M12" s="25" t="e">
+        <v>41932</v>
+      </c>
+      <c r="M12" s="23">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="35" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="31" t="str">
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v/>
       </c>
       <c r="R12" s="8" t="s">
@@ -2006,23 +1964,23 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="23" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>EUR1M</v>
-      </c>
-      <c r="L13" s="24">
+      <c r="K13" s="21" t="str">
+        <f>UPPER(Currency)&amp;"ON"</f>
+        <v>EURON</v>
+      </c>
+      <c r="L13" s="22">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M13" s="25" t="e">
+        <v>41932</v>
+      </c>
+      <c r="M13" s="23">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="36" t="str">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="31" t="str">
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
@@ -2052,7 +2010,7 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="33">
         <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
         <v>41990</v>
       </c>
@@ -2066,23 +2024,23 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="23" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>EUR3M</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="K14" s="21" t="str">
+        <f>UPPER(Currency)&amp;"1M"</f>
+        <v>EUR1M</v>
+      </c>
+      <c r="L14" s="22">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M14" s="25" t="e">
+        <v>41934</v>
+      </c>
+      <c r="M14" s="23">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="36" t="str">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="32" t="str">
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v/>
       </c>
       <c r="R14" s="8" t="s">
@@ -2109,10 +2067,10 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="40" t="b">
+      <c r="B15" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="34">
         <v>42081</v>
       </c>
       <c r="D15" s="8" t="str">
@@ -2124,23 +2082,23 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="23" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>EUR6M</v>
-      </c>
-      <c r="L15" s="24">
+      <c r="K15" s="21" t="str">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>EUR3M</v>
+      </c>
+      <c r="L15" s="22">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M15" s="25" t="e">
+        <v>41934</v>
+      </c>
+      <c r="M15" s="23">
         <f>_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="36" t="str">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <v>1</v>
+      </c>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="32" t="str">
+        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
         <v/>
       </c>
       <c r="R15" s="8" t="s">
@@ -2167,10 +2125,10 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="40" t="b">
+      <c r="B16" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="34">
         <v>42172</v>
       </c>
       <c r="D16" s="8" t="str">
@@ -2182,23 +2140,23 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="43" t="str">
-        <f>UPPER(Currency)&amp;"1Y"</f>
-        <v>EUR1Y</v>
-      </c>
-      <c r="L16" s="44">
+      <c r="K16" s="21" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>EUR6M</v>
+      </c>
+      <c r="L16" s="22">
         <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M16" s="45" t="e">
+        <v>41934</v>
+      </c>
+      <c r="M16" s="23">
         <f>_xll.qlYieldTSDiscount(K16,L16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="46" t="str">
-        <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
+        <v>1</v>
+      </c>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="32" t="str">
+        <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
         <v/>
       </c>
       <c r="R16" s="8" t="s">
@@ -2225,10 +2183,10 @@
     </row>
     <row r="17" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="41" t="b">
+      <c r="B17" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="35">
         <v>42263</v>
       </c>
       <c r="D17" s="10" t="str">
@@ -2240,21 +2198,22 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" s="27">
+      <c r="K17" s="39" t="str">
+        <f>UPPER(Currency)&amp;"1Y"</f>
+        <v>EUR1Y</v>
+      </c>
+      <c r="L17" s="40">
         <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M17" s="59">
+        <v>41934</v>
+      </c>
+      <c r="M17" s="41">
         <f>_xll.qlYieldTSDiscount(K17,L17)</f>
         <v>1</v>
       </c>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="60" t="str">
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42" t="str">
         <f>IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
         <v/>
       </c>
@@ -2291,22 +2250,22 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="44">
+      <c r="K18" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="25" t="e">
         <f>_xll.qlTermStructureReferenceDate(K18,Trigger)</f>
-        <v>41933</v>
-      </c>
-      <c r="M18" s="45">
+        <v>#NUM!</v>
+      </c>
+      <c r="M18" s="55" t="e">
         <f>_xll.qlYieldTSDiscount(K18,L18)</f>
-        <v>1</v>
-      </c>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="46" t="str">
-        <f>IF(ISERROR(L18),_xll.ohRangeRetrieveError(L18),_xll.ohRangeRetrieveError(M18))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="56" t="str">
+        <f ca="1">IF(ISERROR(L18),_xll.ohRangeRetrieveError(L18),_xll.ohRangeRetrieveError(M18))</f>
         <v/>
       </c>
       <c r="R18" s="8" t="s">
@@ -2331,7 +2290,7 @@
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
     </row>
-    <row r="19" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2341,15 +2300,26 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="10" t="s">
+      <c r="J19" s="7"/>
+      <c r="K19" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="40" t="e">
+        <f>_xll.qlTermStructureReferenceDate(K19,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M19" s="41" t="e">
+        <f>_xll.qlYieldTSDiscount(K19,L19)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="42" t="str">
+        <f ca="1">IF(ISERROR(L19),_xll.ohRangeRetrieveError(L19),_xll.ohRangeRetrieveError(M19))</f>
+        <v/>
+      </c>
+      <c r="R19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="S19" s="1"/>
@@ -2371,7 +2341,7 @@
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2381,15 +2351,17 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -3301,7 +3273,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="3"/>
+      <c r="R44" s="1"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="1"/>
@@ -3331,14 +3303,14 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
@@ -5449,40 +5421,51 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:36" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J101" s="61"/>
-      <c r="K101" s="61"/>
-      <c r="L101" s="61"/>
-      <c r="M101" s="61"/>
-      <c r="N101" s="61"/>
-      <c r="O101" s="61"/>
-      <c r="P101" s="61"/>
-      <c r="Q101" s="61"/>
-      <c r="R101" s="61"/>
-      <c r="S101" s="61"/>
-    </row>
-    <row r="102" spans="1:36" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J102" s="61"/>
-      <c r="K102" s="61"/>
-      <c r="L102" s="61"/>
-      <c r="M102" s="61"/>
-      <c r="N102" s="61"/>
-      <c r="O102" s="61"/>
-      <c r="P102" s="61"/>
-      <c r="Q102" s="61"/>
-      <c r="R102" s="61"/>
-      <c r="S102" s="61"/>
+    <row r="101" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="57"/>
+    </row>
+    <row r="102" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J102" s="57"/>
+      <c r="K102" s="57"/>
+      <c r="L102" s="57"/>
+      <c r="M102" s="57"/>
+      <c r="N102" s="57"/>
+      <c r="O102" s="57"/>
+      <c r="P102" s="57"/>
+      <c r="Q102" s="57"/>
+      <c r="R102" s="57"/>
+      <c r="S102" s="57"/>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="J103" s="47"/>
-      <c r="K103" s="47"/>
-      <c r="L103" s="47"/>
-      <c r="M103" s="47"/>
-      <c r="N103" s="47"/>
-      <c r="O103" s="47"/>
-      <c r="P103" s="47"/>
-      <c r="Q103" s="47"/>
-      <c r="R103" s="47"/>
+      <c r="J103" s="57"/>
+      <c r="K103" s="57"/>
+      <c r="L103" s="57"/>
+      <c r="M103" s="57"/>
+      <c r="N103" s="57"/>
+      <c r="O103" s="57"/>
+      <c r="P103" s="57"/>
+      <c r="Q103" s="57"/>
+      <c r="R103" s="57"/>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="J104" s="43"/>
+      <c r="K104" s="43"/>
+      <c r="L104" s="43"/>
+      <c r="M104" s="43"/>
+      <c r="N104" s="43"/>
+      <c r="O104" s="43"/>
+      <c r="P104" s="43"/>
+      <c r="Q104" s="43"/>
+      <c r="R104" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>